<commit_message>
Migrated the whole frontend from Streamlit to React
</commit_message>
<xml_diff>
--- a/Yazle_Invoices_List.xlsx
+++ b/Yazle_Invoices_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://napptix-my.sharepoint.com/personal/abhishek_napptix_com/Documents/Codefiles/InoviceTemplatation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B8AE0-5FCA-4487-AAC7-DACE499F0044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{5C2B8AE0-5FCA-4487-AAC7-DACE499F0044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C4DEC0D-AB59-4A1E-BF63-B4FD232EF6C8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3CB1131B-AA79-4882-985F-1ED357448641}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3CB1131B-AA79-4882-985F-1ED357448641}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales Invoices" sheetId="1" r:id="rId1"/>
@@ -918,26 +918,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20B0E2-9DB4-4834-8272-853CC4728AA7}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="64" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="64" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="30.6328125" customWidth="1"/>
+    <col min="5" max="5" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -972,7 +972,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>45931</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>29</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>45931</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>45962</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>45962</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>45962</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>45992</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>45992</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>45992</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>45992</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>73</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>103</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>45992</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>104</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>45992</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>114</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>46023</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>118</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>119</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>45931</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1697,7 +1697,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E25" s="7" t="s">
         <v>51</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E26" s="7" t="s">
         <v>52</v>
       </c>
@@ -1733,17 +1733,17 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="37.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="37.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>45962</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
       <c r="C3" s="2"/>

</xml_diff>